<commit_message>
arrays practise questions done
</commit_message>
<xml_diff>
--- a/dsalgo/src/test/resources/testData/ArrayPractiseQuestionsTestData.xlsx
+++ b/dsalgo/src/test/resources/testData/ArrayPractiseQuestionsTestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdhan\git\dsalgo\dsalgo\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudha\git\dsalgo\dsalgo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7034E52-A26D-4B65-9C70-7E40D473CEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12460"/>
   </bookViews>
   <sheets>
     <sheet name="pythonCode" sheetId="4" r:id="rId1"/>
@@ -85,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -372,20 +371,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5D1F9E-D72B-4F55-8C42-838A6AFA08E5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="95.5546875" customWidth="1"/>
-    <col min="2" max="2" width="43.88671875" customWidth="1"/>
+    <col min="1" max="1" width="95.54296875" customWidth="1"/>
+    <col min="2" max="2" width="43.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -393,7 +392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="145" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -401,7 +400,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="216" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -409,7 +408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -417,7 +416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>

</xml_diff>